<commit_message>
Updates for thesis submissions
</commit_message>
<xml_diff>
--- a/data/cbn_data_master.xlsx
+++ b/data/cbn_data_master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vuw-my.sharepoint.com/personal/beesech_staff_vuw_ac_nz/Documents/Thesis/3_mizerReef/mizerReef/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vuw-my.sharepoint.com/personal/beesech_staff_vuw_ac_nz/Documents/Thesis/345_mizerReef/mizerReef/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="8_{E2D2E520-1DD2-4F54-9EA3-B27F530A1F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11DAE044-B079-4CC0-A53B-5EBFE8F9B1D9}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="8_{E2D2E520-1DD2-4F54-9EA3-B27F530A1F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08611C04-5B8E-4651-B5FD-9AE8E6643632}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5FEA491A-C879-4E6A-A8BB-35635E46EB26}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5FEA491A-C879-4E6A-A8BB-35635E46EB26}"/>
   </bookViews>
   <sheets>
     <sheet name="Functional groups" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="69">
   <si>
     <t>Group Name</t>
   </si>
@@ -191,12 +191,6 @@
     <t>rep_species</t>
   </si>
   <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>inf</t>
-  </si>
-  <si>
     <t>func_group</t>
   </si>
   <si>
@@ -249,6 +243,9 @@
   </si>
   <si>
     <t>#d078ca</t>
+  </si>
+  <si>
+    <t>pisc_grab</t>
   </si>
 </sst>
 </file>
@@ -405,6 +402,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -707,8 +708,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="O11:Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -740,13 +741,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>33</v>
@@ -785,7 +786,7 @@
         <v>41</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>42</v>
@@ -803,7 +804,7 @@
         <v>23</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>20</v>
@@ -840,7 +841,7 @@
         <v>3.01</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R2" s="3" t="b">
         <v>1</v>
@@ -858,7 +859,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>19</v>
@@ -895,7 +896,7 @@
         <v>3.11</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R3" s="3" t="b">
         <v>1</v>
@@ -913,7 +914,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>3</v>
@@ -950,7 +951,7 @@
         <v>3.1</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R4" s="3" t="b">
         <v>1</v>
@@ -968,7 +969,7 @@
         <v>26</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>18</v>
@@ -1005,7 +1006,7 @@
         <v>3.04</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="R5" s="3" t="b">
         <v>0</v>
@@ -1023,7 +1024,7 @@
         <v>46</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>5</v>
@@ -1060,7 +1061,7 @@
         <v>3.03</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="R6" s="3" t="b">
         <v>1</v>
@@ -1078,7 +1079,7 @@
         <v>27</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>6</v>
@@ -1115,7 +1116,7 @@
         <v>3.24</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="R7" s="3" t="b">
         <v>1</v>
@@ -1133,7 +1134,7 @@
         <v>28</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>8</v>
@@ -1170,7 +1171,7 @@
         <v>2.93</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="R8" s="3" t="b">
         <v>1</v>
@@ -1188,7 +1189,7 @@
         <v>29</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>10</v>
@@ -1225,7 +1226,7 @@
         <v>2.97</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R9" s="3" t="b">
         <v>1</v>
@@ -1243,7 +1244,7 @@
         <v>30</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>12</v>
@@ -1280,7 +1281,7 @@
         <v>2.88</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="R10" s="3" t="b">
         <v>1</v>
@@ -1298,7 +1299,7 @@
         <v>31</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>14</v>
@@ -1335,7 +1336,7 @@
         <v>3</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="R11" s="3" t="b">
         <v>0</v>
@@ -1352,10 +1353,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E93C865-07DA-4F94-BFB8-844F22E994D4}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,20 +1369,19 @@
     <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1407,36 +1407,33 @@
         <v>37</v>
       </c>
       <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="J1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O1" t="s">
-        <v>49</v>
-      </c>
-      <c r="P1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="B2">
         <v>80</v>
@@ -1459,35 +1456,32 @@
       <c r="H2" s="3">
         <v>200</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3">
+        <v>1.7399999999999999E-2</v>
+      </c>
+      <c r="J2" s="3">
+        <v>3.01</v>
+      </c>
+      <c r="K2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="3">
-        <v>1.7399999999999999E-2</v>
-      </c>
-      <c r="K2" s="3">
-        <v>3.01</v>
-      </c>
-      <c r="L2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="P2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
@@ -1512,35 +1506,32 @@
       <c r="H3" s="3">
         <v>30</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="3">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="J3" s="3">
+        <v>3.11</v>
+      </c>
+      <c r="K3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="J3" s="3">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="K3" s="3">
-        <v>3.11</v>
-      </c>
-      <c r="L3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="M3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="P3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1565,35 +1556,32 @@
       <c r="H4" s="3">
         <v>80</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="3">
+        <v>1.2E-2</v>
+      </c>
+      <c r="J4" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="K4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="J4" s="3">
-        <v>1.2E-2</v>
-      </c>
-      <c r="K4" s="3">
-        <v>3.1</v>
-      </c>
-      <c r="L4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="M4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="P4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -1618,35 +1606,32 @@
       <c r="H5" s="3">
         <v>0.25</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="3">
+        <v>1.1220000000000001E-2</v>
+      </c>
+      <c r="J5" s="3">
+        <v>3.04</v>
+      </c>
+      <c r="K5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="J5" s="3">
-        <v>1.1220000000000001E-2</v>
-      </c>
-      <c r="K5" s="3">
-        <v>3.04</v>
-      </c>
-      <c r="L5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="M5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="P5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q5" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1671,35 +1656,32 @@
       <c r="H6" s="3">
         <v>350</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="3">
+        <v>1.259E-2</v>
+      </c>
+      <c r="J6" s="3">
+        <v>3.03</v>
+      </c>
+      <c r="K6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="J6" s="3">
-        <v>1.259E-2</v>
-      </c>
-      <c r="K6" s="3">
-        <v>3.03</v>
-      </c>
-      <c r="L6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="M6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="P6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1724,35 +1706,32 @@
       <c r="H7" s="3">
         <v>0.57499999999999996</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="3">
+        <v>9.7999999999999997E-4</v>
+      </c>
+      <c r="J7" s="3">
+        <v>3.24</v>
+      </c>
+      <c r="K7" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="J7" s="3">
-        <v>9.7999999999999997E-4</v>
-      </c>
-      <c r="K7" s="3">
-        <v>3.24</v>
-      </c>
-      <c r="L7" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="M7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="P7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q7" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -1777,35 +1756,32 @@
       <c r="H8" s="3">
         <v>240</v>
       </c>
-      <c r="I8">
-        <v>20</v>
+      <c r="I8" s="3">
+        <v>2.5700000000000001E-2</v>
       </c>
       <c r="J8" s="3">
-        <v>2.5700000000000001E-2</v>
-      </c>
-      <c r="K8" s="3">
         <v>2.93</v>
       </c>
+      <c r="K8" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="L8" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="M8" s="3" t="b">
-        <v>1</v>
+      <c r="M8" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -1830,35 +1806,32 @@
       <c r="H9" s="3">
         <v>8.5</v>
       </c>
-      <c r="I9">
-        <v>20</v>
+      <c r="I9" s="3">
+        <v>2.0420000000000001E-2</v>
       </c>
       <c r="J9" s="3">
-        <v>2.0420000000000001E-2</v>
-      </c>
-      <c r="K9" s="3">
         <v>2.97</v>
       </c>
+      <c r="K9" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="L9" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="M9" s="3" t="b">
-        <v>1</v>
+      <c r="M9" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1883,35 +1856,32 @@
       <c r="H10" s="3">
         <v>10.4</v>
       </c>
-      <c r="I10">
-        <v>20</v>
+      <c r="I10" s="3">
+        <v>3.236E-2</v>
       </c>
       <c r="J10" s="3">
-        <v>3.236E-2</v>
-      </c>
-      <c r="K10" s="3">
         <v>2.88</v>
       </c>
+      <c r="K10" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="L10" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="M10" s="3" t="b">
-        <v>1</v>
+      <c r="M10" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q10" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
@@ -1936,31 +1906,28 @@
       <c r="H11" s="3">
         <v>100</v>
       </c>
-      <c r="I11">
-        <v>20</v>
+      <c r="I11" s="3">
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="J11" s="3">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="K11" s="3">
         <v>3</v>
       </c>
+      <c r="K11" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="L11" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="M11" s="3" t="b">
-        <v>0</v>
+      <c r="M11" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q11" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1976,407 +1943,407 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2393,7 +2360,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2414,111 +2381,111 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>0.3</v>
+      </c>
+      <c r="C8">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B9">
+        <v>0.5</v>
+      </c>
+      <c r="C9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4">
-        <v>0.3</v>
-      </c>
-      <c r="C4">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>0.5</v>
-      </c>
-      <c r="C6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>0</v>

</xml_diff>